<commit_message>
A 1 to haun stage data to include first leaf
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/Lincoln2021.xlsx
+++ b/Tests/Validation/Wheat/Lincoln2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515294E8-AE4F-42A2-8EB7-B9452D725BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A915150C-3998-4ECB-A755-ABC536414160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,22 @@
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$D$1:$D$1500</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$G$1:$G$1500</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1030,10 +1043,10 @@
   <dimension ref="A1:U1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,7 +1181,7 @@
         <v>0.34599999999999997</v>
       </c>
       <c r="G4">
-        <v>2.9</v>
+        <v>3.9</v>
       </c>
       <c r="H4">
         <v>25</v>
@@ -1223,7 +1236,7 @@
         <v>44294</v>
       </c>
       <c r="G6">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -1281,7 +1294,7 @@
         <v>44301</v>
       </c>
       <c r="G8">
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -1301,7 +1314,7 @@
         <v>44303</v>
       </c>
       <c r="G9">
-        <v>6.7</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -1321,7 +1334,7 @@
         <v>44306</v>
       </c>
       <c r="G10">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1341,7 +1354,7 @@
         <v>44311</v>
       </c>
       <c r="G11">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -1361,7 +1374,7 @@
         <v>44314</v>
       </c>
       <c r="G12">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -1381,7 +1394,7 @@
         <v>44316</v>
       </c>
       <c r="G13">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -1401,7 +1414,7 @@
         <v>44322</v>
       </c>
       <c r="G14">
-        <v>7.7</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -1459,7 +1472,7 @@
         <v>44327</v>
       </c>
       <c r="G16">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1479,7 +1492,7 @@
         <v>44332</v>
       </c>
       <c r="G17">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1499,7 +1512,7 @@
         <v>44335</v>
       </c>
       <c r="G18">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2278,7 +2291,7 @@
         <v>44294</v>
       </c>
       <c r="G58">
-        <v>0.9</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.3">
@@ -2298,7 +2311,7 @@
         <v>44301</v>
       </c>
       <c r="G59">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.3">
@@ -2318,7 +2331,7 @@
         <v>44303</v>
       </c>
       <c r="G60">
-        <v>2.7</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.3">
@@ -2338,7 +2351,7 @@
         <v>44306</v>
       </c>
       <c r="G61">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.3">
@@ -2393,7 +2406,7 @@
         <v>44311</v>
       </c>
       <c r="G63">
-        <v>3.6</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.3">
@@ -2413,7 +2426,7 @@
         <v>44314</v>
       </c>
       <c r="G64">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.3">
@@ -2433,7 +2446,7 @@
         <v>44316</v>
       </c>
       <c r="G65">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.3">
@@ -2453,7 +2466,7 @@
         <v>44322</v>
       </c>
       <c r="G66">
-        <v>4.3</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.3">
@@ -2473,7 +2486,7 @@
         <v>44327</v>
       </c>
       <c r="G67">
-        <v>4.5999999999999996</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.3">
@@ -2493,7 +2506,7 @@
         <v>44332</v>
       </c>
       <c r="G68">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.3">
@@ -2513,7 +2526,7 @@
         <v>44335</v>
       </c>
       <c r="G69">
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.3">
@@ -2571,7 +2584,7 @@
         <v>44337</v>
       </c>
       <c r="G71">
-        <v>5.3</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.3">
@@ -2591,7 +2604,7 @@
         <v>44342</v>
       </c>
       <c r="G72">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.3">
@@ -2611,7 +2624,7 @@
         <v>44345</v>
       </c>
       <c r="G73">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.3">
@@ -2631,7 +2644,7 @@
         <v>44352</v>
       </c>
       <c r="G74">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.3">
@@ -2651,7 +2664,7 @@
         <v>44355</v>
       </c>
       <c r="G75">
-        <v>6.2</v>
+        <v>7.2</v>
       </c>
       <c r="I75" t="s">
         <v>16</v>
@@ -2712,7 +2725,7 @@
         <v>44358</v>
       </c>
       <c r="G77">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.3">
@@ -2732,7 +2745,7 @@
         <v>44363</v>
       </c>
       <c r="G78">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.3">
@@ -2752,7 +2765,7 @@
         <v>44369</v>
       </c>
       <c r="G79">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.3">
@@ -2772,7 +2785,7 @@
         <v>44374</v>
       </c>
       <c r="G80">
-        <v>7.2</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -2792,7 +2805,7 @@
         <v>44377</v>
       </c>
       <c r="G81">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -2812,7 +2825,7 @@
         <v>44380</v>
       </c>
       <c r="G82">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -2832,7 +2845,7 @@
         <v>44384</v>
       </c>
       <c r="G83">
-        <v>7.4</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -2852,7 +2865,7 @@
         <v>44386</v>
       </c>
       <c r="G84">
-        <v>7.4</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -2872,7 +2885,7 @@
         <v>44389</v>
       </c>
       <c r="G85">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -2892,7 +2905,7 @@
         <v>44397</v>
       </c>
       <c r="G86">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -2912,7 +2925,7 @@
         <v>44400</v>
       </c>
       <c r="G87">
-        <v>7.8</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -2932,7 +2945,7 @@
         <v>44405</v>
       </c>
       <c r="G88">
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -2952,7 +2965,7 @@
         <v>44407</v>
       </c>
       <c r="G89">
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -2972,7 +2985,7 @@
         <v>44410</v>
       </c>
       <c r="G90">
-        <v>8.3000000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -2992,7 +3005,7 @@
         <v>44418</v>
       </c>
       <c r="G91">
-        <v>8.4</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3012,7 +3025,7 @@
         <v>44425</v>
       </c>
       <c r="G92">
-        <v>8.4</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3032,7 +3045,7 @@
         <v>44441</v>
       </c>
       <c r="G93">
-        <v>9.1999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3052,7 +3065,7 @@
         <v>44446</v>
       </c>
       <c r="G94">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3072,7 +3085,7 @@
         <v>44451</v>
       </c>
       <c r="G95">
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -3092,7 +3105,7 @@
         <v>44455</v>
       </c>
       <c r="G96">
-        <v>9.6999999999999993</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.3">
@@ -3112,7 +3125,7 @@
         <v>44460</v>
       </c>
       <c r="G97">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.3">
@@ -3132,7 +3145,7 @@
         <v>44463</v>
       </c>
       <c r="G98">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.3">
@@ -3152,7 +3165,7 @@
         <v>44467</v>
       </c>
       <c r="G99">
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.3">
@@ -3172,7 +3185,7 @@
         <v>44471</v>
       </c>
       <c r="G100">
-        <v>10.3</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.3">
@@ -3192,7 +3205,7 @@
         <v>44477</v>
       </c>
       <c r="G101">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.3">
@@ -3273,7 +3286,7 @@
         <v>44489</v>
       </c>
       <c r="G104">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.3">
@@ -3504,7 +3517,7 @@
         <v>44330</v>
       </c>
       <c r="G113">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.3">
@@ -3524,7 +3537,7 @@
         <v>44335</v>
       </c>
       <c r="G114">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.3">
@@ -3544,7 +3557,7 @@
         <v>44337</v>
       </c>
       <c r="G115">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.3">
@@ -3564,7 +3577,7 @@
         <v>44342</v>
       </c>
       <c r="G116">
-        <v>1.9</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.3">
@@ -3584,7 +3597,7 @@
         <v>44345</v>
       </c>
       <c r="G117">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.3">
@@ -3604,7 +3617,7 @@
         <v>44350</v>
       </c>
       <c r="G118">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.3">
@@ -3624,7 +3637,7 @@
         <v>44355</v>
       </c>
       <c r="G119">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.3">
@@ -3682,7 +3695,7 @@
         <v>44358</v>
       </c>
       <c r="G121">
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.3">
@@ -3702,7 +3715,7 @@
         <v>44362</v>
       </c>
       <c r="G122">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.3">
@@ -3722,7 +3735,7 @@
         <v>44369</v>
       </c>
       <c r="G123">
-        <v>3.9</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.3">
@@ -3742,7 +3755,7 @@
         <v>44374</v>
       </c>
       <c r="G124">
-        <v>4.3</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.3">
@@ -3762,7 +3775,7 @@
         <v>44377</v>
       </c>
       <c r="G125">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.3">
@@ -3782,7 +3795,7 @@
         <v>44380</v>
       </c>
       <c r="G126">
-        <v>4.7</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.3">
@@ -3802,7 +3815,7 @@
         <v>44384</v>
       </c>
       <c r="G127">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.3">
@@ -3822,7 +3835,7 @@
         <v>44387</v>
       </c>
       <c r="G128">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.3">
@@ -3880,7 +3893,7 @@
         <v>44390</v>
       </c>
       <c r="G130">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.3">
@@ -3900,7 +3913,7 @@
         <v>44398</v>
       </c>
       <c r="G131">
-        <v>5.3</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.3">
@@ -3920,7 +3933,7 @@
         <v>44403</v>
       </c>
       <c r="G132">
-        <v>5.7</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.3">
@@ -3940,7 +3953,7 @@
         <v>44407</v>
       </c>
       <c r="G133">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.3">
@@ -3960,7 +3973,7 @@
         <v>44412</v>
       </c>
       <c r="G134">
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.3">
@@ -3980,7 +3993,7 @@
         <v>44418</v>
       </c>
       <c r="G135">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.3">
@@ -4000,7 +4013,7 @@
         <v>44425</v>
       </c>
       <c r="G136">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.3">
@@ -4020,7 +4033,7 @@
         <v>44441</v>
       </c>
       <c r="G137">
-        <v>7.8</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.3">
@@ -4078,7 +4091,7 @@
         <v>44446</v>
       </c>
       <c r="G139">
-        <v>8.1999999999999993</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="I139" t="s">
         <v>16</v>
@@ -4101,7 +4114,7 @@
         <v>44451</v>
       </c>
       <c r="G140">
-        <v>8.4</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.3">
@@ -4121,7 +4134,7 @@
         <v>44455</v>
       </c>
       <c r="G141">
-        <v>8.6999999999999993</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.3">
@@ -4141,7 +4154,7 @@
         <v>44460</v>
       </c>
       <c r="G142">
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.3">
@@ -4161,7 +4174,7 @@
         <v>44463</v>
       </c>
       <c r="G143">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.3">
@@ -4181,7 +4194,7 @@
         <v>44467</v>
       </c>
       <c r="G144">
-        <v>9.4</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.3">
@@ -4201,7 +4214,7 @@
         <v>44471</v>
       </c>
       <c r="G145">
-        <v>9.6999999999999993</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.3">
@@ -4221,7 +4234,7 @@
         <v>44477</v>
       </c>
       <c r="G146">
-        <v>10.3</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="147" spans="1:20" x14ac:dyDescent="0.3">
@@ -4241,7 +4254,7 @@
         <v>44489</v>
       </c>
       <c r="G147">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.3">
@@ -4261,7 +4274,7 @@
         <v>44491</v>
       </c>
       <c r="G148">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.3">
@@ -4284,7 +4297,7 @@
         <v>10.718999999999999</v>
       </c>
       <c r="G149">
-        <v>12.2</v>
+        <v>13.2</v>
       </c>
       <c r="H149">
         <v>40</v>
@@ -4553,7 +4566,7 @@
         <v>44379</v>
       </c>
       <c r="G159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.3">
@@ -4573,7 +4586,7 @@
         <v>44384</v>
       </c>
       <c r="G160">
-        <v>0.3</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.3">
@@ -4593,7 +4606,7 @@
         <v>44387</v>
       </c>
       <c r="G161">
-        <v>0.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.3">
@@ -4613,7 +4626,7 @@
         <v>44390</v>
       </c>
       <c r="G162">
-        <v>0.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.3">
@@ -4633,7 +4646,7 @@
         <v>44398</v>
       </c>
       <c r="G163">
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.3">
@@ -4653,7 +4666,7 @@
         <v>44403</v>
       </c>
       <c r="G164">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.3">
@@ -4673,7 +4686,7 @@
         <v>44407</v>
       </c>
       <c r="G165">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.3">
@@ -4728,7 +4741,7 @@
         <v>44412</v>
       </c>
       <c r="G167">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.3">
@@ -4748,7 +4761,7 @@
         <v>44418</v>
       </c>
       <c r="G168">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.3">
@@ -4768,7 +4781,7 @@
         <v>44425</v>
       </c>
       <c r="G169">
-        <v>3.4</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.3">
@@ -4788,7 +4801,7 @@
         <v>44441</v>
       </c>
       <c r="G170">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.3">
@@ -4808,7 +4821,7 @@
         <v>44446</v>
       </c>
       <c r="G171">
-        <v>5.3</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.3">
@@ -4828,7 +4841,7 @@
         <v>44451</v>
       </c>
       <c r="G172">
-        <v>5.6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.3">
@@ -4848,7 +4861,7 @@
         <v>44455</v>
       </c>
       <c r="G173">
-        <v>5.7</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.3">
@@ -4906,7 +4919,7 @@
         <v>44460</v>
       </c>
       <c r="G175">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.3">
@@ -4926,7 +4939,7 @@
         <v>44463</v>
       </c>
       <c r="G176">
-        <v>6.6</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="177" spans="1:20" x14ac:dyDescent="0.3">
@@ -4946,7 +4959,7 @@
         <v>44467</v>
       </c>
       <c r="G177">
-        <v>6.7</v>
+        <v>7.7</v>
       </c>
       <c r="I177" t="s">
         <v>16</v>
@@ -4969,7 +4982,7 @@
         <v>44471</v>
       </c>
       <c r="G178">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="179" spans="1:20" x14ac:dyDescent="0.3">
@@ -4989,7 +5002,7 @@
         <v>44477</v>
       </c>
       <c r="G179">
-        <v>7.7</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.3">
@@ -5047,7 +5060,7 @@
         <v>44489</v>
       </c>
       <c r="G181">
-        <v>9.1999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="182" spans="1:20" x14ac:dyDescent="0.3">
@@ -5067,7 +5080,7 @@
         <v>44491</v>
       </c>
       <c r="G182">
-        <v>9.1999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.3">
@@ -5087,7 +5100,7 @@
         <v>44496</v>
       </c>
       <c r="G183">
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="184" spans="1:20" x14ac:dyDescent="0.3">
@@ -5107,7 +5120,7 @@
         <v>44499</v>
       </c>
       <c r="G184">
-        <v>10.3</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="185" spans="1:20" x14ac:dyDescent="0.3">
@@ -5127,7 +5140,7 @@
         <v>44503</v>
       </c>
       <c r="G185">
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
       <c r="I185" t="s">
         <v>17</v>
@@ -5188,7 +5201,7 @@
         <v>44508</v>
       </c>
       <c r="G187">
-        <v>11.2</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="188" spans="1:20" x14ac:dyDescent="0.3">
@@ -5434,7 +5447,7 @@
         <v>44281</v>
       </c>
       <c r="G196">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="197" spans="1:20" x14ac:dyDescent="0.3">
@@ -5454,7 +5467,7 @@
         <v>44294</v>
       </c>
       <c r="G197">
-        <v>4.7</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="198" spans="1:20" x14ac:dyDescent="0.3">
@@ -5474,7 +5487,7 @@
         <v>44301</v>
       </c>
       <c r="G198">
-        <v>5.6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="199" spans="1:20" x14ac:dyDescent="0.3">
@@ -5494,7 +5507,7 @@
         <v>44303</v>
       </c>
       <c r="G199">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="200" spans="1:20" x14ac:dyDescent="0.3">
@@ -5514,7 +5527,7 @@
         <v>44306</v>
       </c>
       <c r="G200">
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="201" spans="1:20" x14ac:dyDescent="0.3">
@@ -5534,7 +5547,7 @@
         <v>44311</v>
       </c>
       <c r="G201">
-        <v>6.7</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="202" spans="1:20" x14ac:dyDescent="0.3">
@@ -5554,7 +5567,7 @@
         <v>44314</v>
       </c>
       <c r="G202">
-        <v>6.7</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="203" spans="1:20" x14ac:dyDescent="0.3">
@@ -5574,7 +5587,7 @@
         <v>44316</v>
       </c>
       <c r="G203">
-        <v>7.2</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.3">
@@ -5594,7 +5607,7 @@
         <v>44322</v>
       </c>
       <c r="G204">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="205" spans="1:20" x14ac:dyDescent="0.3">
@@ -5614,7 +5627,7 @@
         <v>44327</v>
       </c>
       <c r="G205">
-        <v>7.9</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="206" spans="1:20" x14ac:dyDescent="0.3">
@@ -5634,7 +5647,7 @@
         <v>44332</v>
       </c>
       <c r="G206">
-        <v>8.3000000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.3">
@@ -5654,7 +5667,7 @@
         <v>44335</v>
       </c>
       <c r="G207">
-        <v>8.3000000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="208" spans="1:20" x14ac:dyDescent="0.3">
@@ -5712,7 +5725,7 @@
         <v>44337</v>
       </c>
       <c r="G209">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
@@ -5732,7 +5745,7 @@
         <v>44342</v>
       </c>
       <c r="G210">
-        <v>8.6999999999999993</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
@@ -5752,7 +5765,7 @@
         <v>44345</v>
       </c>
       <c r="G211">
-        <v>8.6999999999999993</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
@@ -5792,7 +5805,7 @@
         <v>44352</v>
       </c>
       <c r="G213">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
@@ -5812,7 +5825,7 @@
         <v>44356</v>
       </c>
       <c r="G214">
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
@@ -5832,7 +5845,7 @@
         <v>44359</v>
       </c>
       <c r="G215">
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
@@ -5852,7 +5865,7 @@
         <v>44363</v>
       </c>
       <c r="G216">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
@@ -5872,7 +5885,7 @@
         <v>44369</v>
       </c>
       <c r="G217">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
@@ -5892,7 +5905,7 @@
         <v>44372</v>
       </c>
       <c r="G218">
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
@@ -5912,7 +5925,7 @@
         <v>44375</v>
       </c>
       <c r="G219">
-        <v>10.3</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
@@ -5932,7 +5945,7 @@
         <v>44379</v>
       </c>
       <c r="G220">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
@@ -5952,7 +5965,7 @@
         <v>44384</v>
       </c>
       <c r="G221">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
@@ -5972,7 +5985,7 @@
         <v>44386</v>
       </c>
       <c r="G222">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
@@ -5992,7 +6005,7 @@
         <v>44389</v>
       </c>
       <c r="G223">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
@@ -6012,7 +6025,7 @@
         <v>44397</v>
       </c>
       <c r="G224">
-        <v>10.7</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="225" spans="1:20" x14ac:dyDescent="0.3">
@@ -6070,7 +6083,7 @@
         <v>44400</v>
       </c>
       <c r="G226">
-        <v>10.9</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.3">
@@ -6090,7 +6103,7 @@
         <v>44405</v>
       </c>
       <c r="G227">
-        <v>11.2</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.3">
@@ -6110,7 +6123,7 @@
         <v>44407</v>
       </c>
       <c r="G228">
-        <v>11.2</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.3">
@@ -6130,7 +6143,7 @@
         <v>44410</v>
       </c>
       <c r="G229">
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="230" spans="1:20" x14ac:dyDescent="0.3">
@@ -6150,7 +6163,7 @@
         <v>44418</v>
       </c>
       <c r="G230">
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="231" spans="1:20" x14ac:dyDescent="0.3">
@@ -6170,7 +6183,7 @@
         <v>44425</v>
       </c>
       <c r="G231">
-        <v>11.8</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="232" spans="1:20" x14ac:dyDescent="0.3">
@@ -6190,7 +6203,7 @@
         <v>44441</v>
       </c>
       <c r="G232">
-        <v>12.8</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="233" spans="1:20" x14ac:dyDescent="0.3">
@@ -6210,7 +6223,7 @@
         <v>44446</v>
       </c>
       <c r="G233">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="234" spans="1:20" x14ac:dyDescent="0.3">
@@ -6230,7 +6243,7 @@
         <v>44451</v>
       </c>
       <c r="G234">
-        <v>13.4</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="235" spans="1:20" x14ac:dyDescent="0.3">
@@ -6250,7 +6263,7 @@
         <v>44455</v>
       </c>
       <c r="G235">
-        <v>13.7</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="236" spans="1:20" x14ac:dyDescent="0.3">
@@ -6270,7 +6283,7 @@
         <v>44460</v>
       </c>
       <c r="G236">
-        <v>13.8</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="237" spans="1:20" x14ac:dyDescent="0.3">
@@ -6290,7 +6303,7 @@
         <v>44463</v>
       </c>
       <c r="G237">
-        <v>14.2</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="238" spans="1:20" x14ac:dyDescent="0.3">
@@ -6310,7 +6323,7 @@
         <v>44467</v>
       </c>
       <c r="G238">
-        <v>14.3</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="239" spans="1:20" x14ac:dyDescent="0.3">
@@ -6330,7 +6343,7 @@
         <v>44471</v>
       </c>
       <c r="G239">
-        <v>14.7</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="240" spans="1:20" x14ac:dyDescent="0.3">
@@ -6350,7 +6363,7 @@
         <v>44477</v>
       </c>
       <c r="G240">
-        <v>15.2</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="241" spans="1:20" x14ac:dyDescent="0.3">
@@ -6428,7 +6441,7 @@
         <v>44489</v>
       </c>
       <c r="G243">
-        <v>16.2</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.3">
@@ -6639,7 +6652,7 @@
         <v>44294</v>
       </c>
       <c r="G251">
-        <v>0.3</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="252" spans="1:20" x14ac:dyDescent="0.3">
@@ -6659,7 +6672,7 @@
         <v>44301</v>
       </c>
       <c r="G252">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="253" spans="1:20" x14ac:dyDescent="0.3">
@@ -6679,7 +6692,7 @@
         <v>44303</v>
       </c>
       <c r="G253">
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="254" spans="1:20" x14ac:dyDescent="0.3">
@@ -6699,7 +6712,7 @@
         <v>44306</v>
       </c>
       <c r="G254">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="255" spans="1:20" x14ac:dyDescent="0.3">
@@ -6754,7 +6767,7 @@
         <v>44311</v>
       </c>
       <c r="G256">
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.3">
@@ -6774,7 +6787,7 @@
         <v>44314</v>
       </c>
       <c r="G257">
-        <v>3.4</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.3">
@@ -6794,7 +6807,7 @@
         <v>44316</v>
       </c>
       <c r="G258">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.3">
@@ -6814,7 +6827,7 @@
         <v>44322</v>
       </c>
       <c r="G259">
-        <v>4.3</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.3">
@@ -6834,7 +6847,7 @@
         <v>44327</v>
       </c>
       <c r="G260">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.3">
@@ -6854,7 +6867,7 @@
         <v>44332</v>
       </c>
       <c r="G261">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="262" spans="1:20" x14ac:dyDescent="0.3">
@@ -6874,7 +6887,7 @@
         <v>44335</v>
       </c>
       <c r="G262">
-        <v>5.7</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="263" spans="1:20" x14ac:dyDescent="0.3">
@@ -6894,7 +6907,7 @@
         <v>44337</v>
       </c>
       <c r="G263">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="264" spans="1:20" x14ac:dyDescent="0.3">
@@ -6917,7 +6930,7 @@
         <v>2.673</v>
       </c>
       <c r="G264">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
       <c r="H264">
         <v>30</v>
@@ -6955,7 +6968,7 @@
         <v>44345</v>
       </c>
       <c r="G265">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="266" spans="1:20" x14ac:dyDescent="0.3">
@@ -6975,7 +6988,7 @@
         <v>44352</v>
       </c>
       <c r="G266">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="267" spans="1:20" x14ac:dyDescent="0.3">
@@ -6995,7 +7008,7 @@
         <v>44355</v>
       </c>
       <c r="G267">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="268" spans="1:20" x14ac:dyDescent="0.3">
@@ -7015,7 +7028,7 @@
         <v>44358</v>
       </c>
       <c r="G268">
-        <v>6.9</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="269" spans="1:20" x14ac:dyDescent="0.3">
@@ -7055,7 +7068,7 @@
         <v>44363</v>
       </c>
       <c r="G270">
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="271" spans="1:20" x14ac:dyDescent="0.3">
@@ -7075,7 +7088,7 @@
         <v>44369</v>
       </c>
       <c r="G271">
-        <v>7.8</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="272" spans="1:20" x14ac:dyDescent="0.3">
@@ -7095,7 +7108,7 @@
         <v>44374</v>
       </c>
       <c r="G272">
-        <v>7.8</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="273" spans="1:20" x14ac:dyDescent="0.3">
@@ -7115,7 +7128,7 @@
         <v>44377</v>
       </c>
       <c r="G273">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="274" spans="1:20" x14ac:dyDescent="0.3">
@@ -7135,7 +7148,7 @@
         <v>44380</v>
       </c>
       <c r="G274">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="275" spans="1:20" x14ac:dyDescent="0.3">
@@ -7155,7 +7168,7 @@
         <v>44384</v>
       </c>
       <c r="G275">
-        <v>8.1999999999999993</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="276" spans="1:20" x14ac:dyDescent="0.3">
@@ -7175,7 +7188,7 @@
         <v>44386</v>
       </c>
       <c r="G276">
-        <v>8.1999999999999993</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="277" spans="1:20" x14ac:dyDescent="0.3">
@@ -7195,7 +7208,7 @@
         <v>44389</v>
       </c>
       <c r="G277">
-        <v>8.4</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="278" spans="1:20" x14ac:dyDescent="0.3">
@@ -7215,7 +7228,7 @@
         <v>44397</v>
       </c>
       <c r="G278">
-        <v>8.8000000000000007</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="279" spans="1:20" x14ac:dyDescent="0.3">
@@ -7235,7 +7248,7 @@
         <v>44400</v>
       </c>
       <c r="G279">
-        <v>8.8000000000000007</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="280" spans="1:20" x14ac:dyDescent="0.3">
@@ -7255,7 +7268,7 @@
         <v>44405</v>
       </c>
       <c r="G280">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="281" spans="1:20" x14ac:dyDescent="0.3">
@@ -7275,7 +7288,7 @@
         <v>44407</v>
       </c>
       <c r="G281">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="282" spans="1:20" x14ac:dyDescent="0.3">
@@ -7295,7 +7308,7 @@
         <v>44410</v>
       </c>
       <c r="G282">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="283" spans="1:20" x14ac:dyDescent="0.3">
@@ -7315,7 +7328,7 @@
         <v>44418</v>
       </c>
       <c r="G283">
-        <v>9.6999999999999993</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="284" spans="1:20" x14ac:dyDescent="0.3">
@@ -7373,7 +7386,7 @@
         <v>44425</v>
       </c>
       <c r="G285">
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="286" spans="1:20" x14ac:dyDescent="0.3">
@@ -7393,7 +7406,7 @@
         <v>44441</v>
       </c>
       <c r="G286">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="287" spans="1:20" x14ac:dyDescent="0.3">
@@ -7413,7 +7426,7 @@
         <v>44446</v>
       </c>
       <c r="G287">
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="288" spans="1:20" x14ac:dyDescent="0.3">
@@ -7433,7 +7446,7 @@
         <v>44451</v>
       </c>
       <c r="G288">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="289" spans="1:20" x14ac:dyDescent="0.3">
@@ -7453,7 +7466,7 @@
         <v>44455</v>
       </c>
       <c r="G289">
-        <v>11.6</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="290" spans="1:20" x14ac:dyDescent="0.3">
@@ -7473,7 +7486,7 @@
         <v>44460</v>
       </c>
       <c r="G290">
-        <v>11.8</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="291" spans="1:20" x14ac:dyDescent="0.3">
@@ -7493,7 +7506,7 @@
         <v>44463</v>
       </c>
       <c r="G291">
-        <v>12.2</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="292" spans="1:20" x14ac:dyDescent="0.3">
@@ -7513,7 +7526,7 @@
         <v>44467</v>
       </c>
       <c r="G292">
-        <v>12.3</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="293" spans="1:20" x14ac:dyDescent="0.3">
@@ -7533,7 +7546,7 @@
         <v>44471</v>
       </c>
       <c r="G293">
-        <v>12.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="294" spans="1:20" x14ac:dyDescent="0.3">
@@ -7553,7 +7566,7 @@
         <v>44477</v>
       </c>
       <c r="G294">
-        <v>13.2</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="295" spans="1:20" x14ac:dyDescent="0.3">
@@ -7631,7 +7644,7 @@
         <v>44489</v>
       </c>
       <c r="G297">
-        <v>14.1</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="298" spans="1:20" x14ac:dyDescent="0.3">
@@ -7862,7 +7875,7 @@
         <v>44330</v>
       </c>
       <c r="G306">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="307" spans="1:20" x14ac:dyDescent="0.3">
@@ -7882,7 +7895,7 @@
         <v>44335</v>
       </c>
       <c r="G307">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="308" spans="1:20" x14ac:dyDescent="0.3">
@@ -7902,7 +7915,7 @@
         <v>44337</v>
       </c>
       <c r="G308">
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="309" spans="1:20" x14ac:dyDescent="0.3">
@@ -7922,7 +7935,7 @@
         <v>44342</v>
       </c>
       <c r="G309">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="310" spans="1:20" x14ac:dyDescent="0.3">
@@ -7942,7 +7955,7 @@
         <v>44345</v>
       </c>
       <c r="G310">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="311" spans="1:20" x14ac:dyDescent="0.3">
@@ -7962,7 +7975,7 @@
         <v>44350</v>
       </c>
       <c r="G311">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="312" spans="1:20" x14ac:dyDescent="0.3">
@@ -7982,7 +7995,7 @@
         <v>44355</v>
       </c>
       <c r="G312">
-        <v>2.7</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="313" spans="1:20" x14ac:dyDescent="0.3">
@@ -8040,7 +8053,7 @@
         <v>44358</v>
       </c>
       <c r="G314">
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="315" spans="1:20" x14ac:dyDescent="0.3">
@@ -8060,7 +8073,7 @@
         <v>44362</v>
       </c>
       <c r="G315">
-        <v>3.6</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="316" spans="1:20" x14ac:dyDescent="0.3">
@@ -8080,7 +8093,7 @@
         <v>44369</v>
       </c>
       <c r="G316">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="317" spans="1:20" x14ac:dyDescent="0.3">
@@ -8100,7 +8113,7 @@
         <v>44374</v>
       </c>
       <c r="G317">
-        <v>4.3</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="318" spans="1:20" x14ac:dyDescent="0.3">
@@ -8120,7 +8133,7 @@
         <v>44377</v>
       </c>
       <c r="G318">
-        <v>4.7</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="319" spans="1:20" x14ac:dyDescent="0.3">
@@ -8140,7 +8153,7 @@
         <v>44380</v>
       </c>
       <c r="G319">
-        <v>4.7</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="320" spans="1:20" x14ac:dyDescent="0.3">
@@ -8160,7 +8173,7 @@
         <v>44384</v>
       </c>
       <c r="G320">
-        <v>4.9000000000000004</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="321" spans="1:20" x14ac:dyDescent="0.3">
@@ -8180,7 +8193,7 @@
         <v>44387</v>
       </c>
       <c r="G321">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="322" spans="1:20" x14ac:dyDescent="0.3">
@@ -8200,7 +8213,7 @@
         <v>44390</v>
       </c>
       <c r="G322">
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="323" spans="1:20" x14ac:dyDescent="0.3">
@@ -8220,7 +8233,7 @@
         <v>44398</v>
       </c>
       <c r="G323">
-        <v>5.7</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="324" spans="1:20" x14ac:dyDescent="0.3">
@@ -8240,7 +8253,7 @@
         <v>44403</v>
       </c>
       <c r="G324">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="325" spans="1:20" x14ac:dyDescent="0.3">
@@ -8260,7 +8273,7 @@
         <v>44407</v>
       </c>
       <c r="G325">
-        <v>6.2</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="326" spans="1:20" x14ac:dyDescent="0.3">
@@ -8280,7 +8293,7 @@
         <v>44412</v>
       </c>
       <c r="G326">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="327" spans="1:20" x14ac:dyDescent="0.3">
@@ -8300,7 +8313,7 @@
         <v>44418</v>
       </c>
       <c r="G327">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="328" spans="1:20" x14ac:dyDescent="0.3">
@@ -8320,7 +8333,7 @@
         <v>44425</v>
       </c>
       <c r="G328">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="329" spans="1:20" x14ac:dyDescent="0.3">
@@ -8343,7 +8356,7 @@
         <v>3.9489999999999998</v>
       </c>
       <c r="G329">
-        <v>8.3000000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H329">
         <v>30</v>
@@ -8381,7 +8394,7 @@
         <v>44446</v>
       </c>
       <c r="G330">
-        <v>8.6</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="331" spans="1:20" x14ac:dyDescent="0.3">
@@ -8401,7 +8414,7 @@
         <v>44451</v>
       </c>
       <c r="G331">
-        <v>8.8000000000000007</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="332" spans="1:20" x14ac:dyDescent="0.3">
@@ -8441,7 +8454,7 @@
         <v>44455</v>
       </c>
       <c r="G333">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="334" spans="1:20" x14ac:dyDescent="0.3">
@@ -8499,7 +8512,7 @@
         <v>44460</v>
       </c>
       <c r="G335">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="336" spans="1:20" x14ac:dyDescent="0.3">
@@ -8519,7 +8532,7 @@
         <v>44463</v>
       </c>
       <c r="G336">
-        <v>9.6999999999999993</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="337" spans="1:20" x14ac:dyDescent="0.3">
@@ -8539,7 +8552,7 @@
         <v>44467</v>
       </c>
       <c r="G337">
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="338" spans="1:20" x14ac:dyDescent="0.3">
@@ -8559,7 +8572,7 @@
         <v>44471</v>
       </c>
       <c r="G338">
-        <v>10.3</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="339" spans="1:20" x14ac:dyDescent="0.3">
@@ -8579,7 +8592,7 @@
         <v>44477</v>
       </c>
       <c r="G339">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="340" spans="1:20" x14ac:dyDescent="0.3">
@@ -8599,7 +8612,7 @@
         <v>44489</v>
       </c>
       <c r="G340">
-        <v>11.8</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="341" spans="1:20" x14ac:dyDescent="0.3">
@@ -8619,7 +8632,7 @@
         <v>44491</v>
       </c>
       <c r="G341">
-        <v>11.8</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="342" spans="1:20" x14ac:dyDescent="0.3">
@@ -8642,7 +8655,7 @@
         <v>11.334</v>
       </c>
       <c r="G342">
-        <v>12.7</v>
+        <v>13.7</v>
       </c>
       <c r="H342">
         <v>40</v>
@@ -8911,7 +8924,7 @@
         <v>44379</v>
       </c>
       <c r="G352">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="353" spans="1:20" x14ac:dyDescent="0.3">
@@ -8931,7 +8944,7 @@
         <v>44384</v>
       </c>
       <c r="G353">
-        <v>0.3</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="354" spans="1:20" x14ac:dyDescent="0.3">
@@ -8951,7 +8964,7 @@
         <v>44387</v>
       </c>
       <c r="G354">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="355" spans="1:20" x14ac:dyDescent="0.3">
@@ -8971,7 +8984,7 @@
         <v>44390</v>
       </c>
       <c r="G355">
-        <v>0.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="356" spans="1:20" x14ac:dyDescent="0.3">
@@ -8991,7 +9004,7 @@
         <v>44398</v>
       </c>
       <c r="G356">
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="357" spans="1:20" x14ac:dyDescent="0.3">
@@ -9011,7 +9024,7 @@
         <v>44403</v>
       </c>
       <c r="G357">
-        <v>1.7</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="358" spans="1:20" x14ac:dyDescent="0.3">
@@ -9031,7 +9044,7 @@
         <v>44407</v>
       </c>
       <c r="G358">
-        <v>1.9</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="359" spans="1:20" x14ac:dyDescent="0.3">
@@ -9089,7 +9102,7 @@
         <v>44412</v>
       </c>
       <c r="G360">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="361" spans="1:20" x14ac:dyDescent="0.3">
@@ -9109,7 +9122,7 @@
         <v>44418</v>
       </c>
       <c r="G361">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="362" spans="1:20" x14ac:dyDescent="0.3">
@@ -9129,7 +9142,7 @@
         <v>44425</v>
       </c>
       <c r="G362">
-        <v>3.4</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="363" spans="1:20" x14ac:dyDescent="0.3">
@@ -9149,7 +9162,7 @@
         <v>44441</v>
       </c>
       <c r="G363">
-        <v>4.7</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="364" spans="1:20" x14ac:dyDescent="0.3">
@@ -9169,7 +9182,7 @@
         <v>44446</v>
       </c>
       <c r="G364">
-        <v>5.3</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="365" spans="1:20" x14ac:dyDescent="0.3">
@@ -9189,7 +9202,7 @@
         <v>44451</v>
       </c>
       <c r="G365">
-        <v>5.6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="366" spans="1:20" x14ac:dyDescent="0.3">
@@ -9209,7 +9222,7 @@
         <v>44455</v>
       </c>
       <c r="G366">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="367" spans="1:20" x14ac:dyDescent="0.3">
@@ -9229,7 +9242,7 @@
         <v>44460</v>
       </c>
       <c r="G367">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="368" spans="1:20" x14ac:dyDescent="0.3">
@@ -9252,7 +9265,7 @@
         <v>3.1110000000000002</v>
       </c>
       <c r="G368">
-        <v>6.6</v>
+        <v>7.6</v>
       </c>
       <c r="H368">
         <v>30</v>
@@ -9290,7 +9303,7 @@
         <v>44467</v>
       </c>
       <c r="G369">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="370" spans="1:20" x14ac:dyDescent="0.3">
@@ -9310,7 +9323,7 @@
         <v>44471</v>
       </c>
       <c r="G370">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I370" t="s">
         <v>16</v>
@@ -9333,7 +9346,7 @@
         <v>44477</v>
       </c>
       <c r="G371">
-        <v>7.7</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="372" spans="1:20" x14ac:dyDescent="0.3">
@@ -9391,7 +9404,7 @@
         <v>44489</v>
       </c>
       <c r="G373">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="374" spans="1:20" x14ac:dyDescent="0.3">
@@ -9411,7 +9424,7 @@
         <v>44491</v>
       </c>
       <c r="G374">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="375" spans="1:20" x14ac:dyDescent="0.3">
@@ -9431,7 +9444,7 @@
         <v>44496</v>
       </c>
       <c r="G375">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="376" spans="1:20" x14ac:dyDescent="0.3">
@@ -9451,7 +9464,7 @@
         <v>44499</v>
       </c>
       <c r="G376">
-        <v>10.3</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="377" spans="1:20" x14ac:dyDescent="0.3">
@@ -9471,7 +9484,7 @@
         <v>44503</v>
       </c>
       <c r="G377">
-        <v>10.3</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="378" spans="1:20" x14ac:dyDescent="0.3">
@@ -9529,7 +9542,7 @@
         <v>44508</v>
       </c>
       <c r="G379">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
       <c r="I379" t="s">
         <v>17</v>
@@ -9778,7 +9791,7 @@
         <v>44281</v>
       </c>
       <c r="G388">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="389" spans="1:20" x14ac:dyDescent="0.3">
@@ -9798,7 +9811,7 @@
         <v>44294</v>
       </c>
       <c r="G389">
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="390" spans="1:20" x14ac:dyDescent="0.3">
@@ -9818,7 +9831,7 @@
         <v>44301</v>
       </c>
       <c r="G390">
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="391" spans="1:20" x14ac:dyDescent="0.3">
@@ -9838,7 +9851,7 @@
         <v>44303</v>
       </c>
       <c r="G391">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="392" spans="1:20" x14ac:dyDescent="0.3">
@@ -9858,7 +9871,7 @@
         <v>44306</v>
       </c>
       <c r="G392">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="393" spans="1:20" x14ac:dyDescent="0.3">
@@ -9878,7 +9891,7 @@
         <v>44311</v>
       </c>
       <c r="G393">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="394" spans="1:20" x14ac:dyDescent="0.3">
@@ -9898,7 +9911,7 @@
         <v>44314</v>
       </c>
       <c r="G394">
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="395" spans="1:20" x14ac:dyDescent="0.3">
@@ -9918,7 +9931,7 @@
         <v>44316</v>
       </c>
       <c r="G395">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="396" spans="1:20" x14ac:dyDescent="0.3">
@@ -9938,7 +9951,7 @@
         <v>44322</v>
       </c>
       <c r="G396">
-        <v>7.8</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="397" spans="1:20" x14ac:dyDescent="0.3">
@@ -9958,7 +9971,7 @@
         <v>44327</v>
       </c>
       <c r="G397">
-        <v>8.3000000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="398" spans="1:20" x14ac:dyDescent="0.3">
@@ -9978,7 +9991,7 @@
         <v>44332</v>
       </c>
       <c r="G398">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="399" spans="1:20" x14ac:dyDescent="0.3">
@@ -9998,7 +10011,7 @@
         <v>44335</v>
       </c>
       <c r="G399">
-        <v>8.6999999999999993</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="400" spans="1:20" x14ac:dyDescent="0.3">
@@ -10056,7 +10069,7 @@
         <v>44337</v>
       </c>
       <c r="G401">
-        <v>8.8000000000000007</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="402" spans="1:20" x14ac:dyDescent="0.3">
@@ -10076,7 +10089,7 @@
         <v>44342</v>
       </c>
       <c r="G402">
-        <v>8.9</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="403" spans="1:20" x14ac:dyDescent="0.3">
@@ -10096,7 +10109,7 @@
         <v>44345</v>
       </c>
       <c r="G403">
-        <v>8.9</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="404" spans="1:20" x14ac:dyDescent="0.3">
@@ -10136,7 +10149,7 @@
         <v>44352</v>
       </c>
       <c r="G405">
-        <v>9.4</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="406" spans="1:20" x14ac:dyDescent="0.3">
@@ -10156,7 +10169,7 @@
         <v>44356</v>
       </c>
       <c r="G406">
-        <v>9.6999999999999993</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="407" spans="1:20" x14ac:dyDescent="0.3">
@@ -10176,7 +10189,7 @@
         <v>44359</v>
       </c>
       <c r="G407">
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="408" spans="1:20" x14ac:dyDescent="0.3">
@@ -10196,7 +10209,7 @@
         <v>44363</v>
       </c>
       <c r="G408">
-        <v>10.1</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="409" spans="1:20" x14ac:dyDescent="0.3">
@@ -10219,7 +10232,7 @@
         <v>8.8620000000000001</v>
       </c>
       <c r="G409">
-        <v>10.4</v>
+        <v>11.4</v>
       </c>
       <c r="H409">
         <v>32</v>
@@ -10257,7 +10270,7 @@
         <v>44372</v>
       </c>
       <c r="G410">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="411" spans="1:20" x14ac:dyDescent="0.3">
@@ -10277,7 +10290,7 @@
         <v>44375</v>
       </c>
       <c r="G411">
-        <v>10.9</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="412" spans="1:20" x14ac:dyDescent="0.3">
@@ -10297,7 +10310,7 @@
         <v>44379</v>
       </c>
       <c r="G412">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="413" spans="1:20" x14ac:dyDescent="0.3">
@@ -10317,7 +10330,7 @@
         <v>44384</v>
       </c>
       <c r="G413">
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="414" spans="1:20" x14ac:dyDescent="0.3">
@@ -10337,7 +10350,7 @@
         <v>44386</v>
       </c>
       <c r="G414">
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="415" spans="1:20" x14ac:dyDescent="0.3">
@@ -10357,7 +10370,7 @@
         <v>44389</v>
       </c>
       <c r="G415">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="416" spans="1:20" x14ac:dyDescent="0.3">
@@ -10377,7 +10390,7 @@
         <v>44397</v>
       </c>
       <c r="G416">
-        <v>11.6</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="417" spans="1:9" x14ac:dyDescent="0.3">
@@ -10397,7 +10410,7 @@
         <v>44400</v>
       </c>
       <c r="G417">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="418" spans="1:9" x14ac:dyDescent="0.3">
@@ -10417,7 +10430,7 @@
         <v>44405</v>
       </c>
       <c r="G418">
-        <v>12.2</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="419" spans="1:9" x14ac:dyDescent="0.3">
@@ -10437,7 +10450,7 @@
         <v>44407</v>
       </c>
       <c r="G419">
-        <v>12.3</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="420" spans="1:9" x14ac:dyDescent="0.3">
@@ -10457,7 +10470,7 @@
         <v>44410</v>
       </c>
       <c r="G420">
-        <v>12.4</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="421" spans="1:9" x14ac:dyDescent="0.3">
@@ -10477,7 +10490,7 @@
         <v>44418</v>
       </c>
       <c r="G421">
-        <v>12.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="422" spans="1:9" x14ac:dyDescent="0.3">
@@ -10497,7 +10510,7 @@
         <v>44425</v>
       </c>
       <c r="G422">
-        <v>13.2</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="423" spans="1:9" x14ac:dyDescent="0.3">
@@ -10517,7 +10530,7 @@
         <v>44441</v>
       </c>
       <c r="G423">
-        <v>14.1</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="424" spans="1:9" x14ac:dyDescent="0.3">
@@ -10537,7 +10550,7 @@
         <v>44446</v>
       </c>
       <c r="G424">
-        <v>14.3</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="425" spans="1:9" x14ac:dyDescent="0.3">
@@ -10557,7 +10570,7 @@
         <v>44451</v>
       </c>
       <c r="G425">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="426" spans="1:9" x14ac:dyDescent="0.3">
@@ -10577,7 +10590,7 @@
         <v>44455</v>
       </c>
       <c r="G426">
-        <v>14.6</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.3">
@@ -10597,7 +10610,7 @@
         <v>44460</v>
       </c>
       <c r="G427">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="428" spans="1:9" x14ac:dyDescent="0.3">
@@ -10617,7 +10630,7 @@
         <v>44463</v>
       </c>
       <c r="G428">
-        <v>15.2</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="429" spans="1:9" x14ac:dyDescent="0.3">
@@ -10637,7 +10650,7 @@
         <v>44467</v>
       </c>
       <c r="G429">
-        <v>15.3</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="430" spans="1:9" x14ac:dyDescent="0.3">
@@ -10657,7 +10670,7 @@
         <v>44471</v>
       </c>
       <c r="G430">
-        <v>15.4</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="431" spans="1:9" x14ac:dyDescent="0.3">
@@ -10677,7 +10690,7 @@
         <v>44477</v>
       </c>
       <c r="G431">
-        <v>15.8</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="432" spans="1:9" x14ac:dyDescent="0.3">
@@ -10755,7 +10768,7 @@
         <v>44489</v>
       </c>
       <c r="G434">
-        <v>16.399999999999999</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="435" spans="1:20" x14ac:dyDescent="0.3">
@@ -10966,7 +10979,7 @@
         <v>44294</v>
       </c>
       <c r="G442">
-        <v>0.75</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="443" spans="1:20" x14ac:dyDescent="0.3">
@@ -10986,7 +10999,7 @@
         <v>44301</v>
       </c>
       <c r="G443">
-        <v>1.78</v>
+        <v>2.7800000000000002</v>
       </c>
     </row>
     <row r="444" spans="1:20" x14ac:dyDescent="0.3">
@@ -11006,7 +11019,7 @@
         <v>44303</v>
       </c>
       <c r="G444">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="445" spans="1:20" x14ac:dyDescent="0.3">
@@ -11026,7 +11039,7 @@
         <v>44306</v>
       </c>
       <c r="G445">
-        <v>2.83</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="446" spans="1:20" x14ac:dyDescent="0.3">
@@ -11081,7 +11094,7 @@
         <v>44311</v>
       </c>
       <c r="G447">
-        <v>3.42</v>
+        <v>4.42</v>
       </c>
     </row>
     <row r="448" spans="1:20" x14ac:dyDescent="0.3">
@@ -11101,7 +11114,7 @@
         <v>44314</v>
       </c>
       <c r="G448">
-        <v>3.92</v>
+        <v>4.92</v>
       </c>
     </row>
     <row r="449" spans="1:20" x14ac:dyDescent="0.3">
@@ -11121,7 +11134,7 @@
         <v>44316</v>
       </c>
       <c r="G449">
-        <v>3.92</v>
+        <v>4.92</v>
       </c>
     </row>
     <row r="450" spans="1:20" x14ac:dyDescent="0.3">
@@ -11141,7 +11154,7 @@
         <v>44322</v>
       </c>
       <c r="G450">
-        <v>4.75</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="451" spans="1:20" x14ac:dyDescent="0.3">
@@ -11161,7 +11174,7 @@
         <v>44327</v>
       </c>
       <c r="G451">
-        <v>5.1100000000000003</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="452" spans="1:20" x14ac:dyDescent="0.3">
@@ -11181,7 +11194,7 @@
         <v>44332</v>
       </c>
       <c r="G452">
-        <v>5.67</v>
+        <v>6.67</v>
       </c>
     </row>
     <row r="453" spans="1:20" x14ac:dyDescent="0.3">
@@ -11201,7 +11214,7 @@
         <v>44335</v>
       </c>
       <c r="G453">
-        <v>5.75</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="454" spans="1:20" x14ac:dyDescent="0.3">
@@ -11221,7 +11234,7 @@
         <v>44337</v>
       </c>
       <c r="G454">
-        <v>5.92</v>
+        <v>6.92</v>
       </c>
     </row>
     <row r="455" spans="1:20" x14ac:dyDescent="0.3">
@@ -11244,7 +11257,7 @@
         <v>3.347</v>
       </c>
       <c r="G455">
-        <v>5.92</v>
+        <v>6.92</v>
       </c>
       <c r="H455">
         <v>30</v>
@@ -11282,7 +11295,7 @@
         <v>44345</v>
       </c>
       <c r="G456">
-        <v>6.08</v>
+        <v>7.08</v>
       </c>
     </row>
     <row r="457" spans="1:20" x14ac:dyDescent="0.3">
@@ -11302,7 +11315,7 @@
         <v>44352</v>
       </c>
       <c r="G457">
-        <v>6.67</v>
+        <v>7.67</v>
       </c>
     </row>
     <row r="458" spans="1:20" x14ac:dyDescent="0.3">
@@ -11322,7 +11335,7 @@
         <v>44355</v>
       </c>
       <c r="G458">
-        <v>6.92</v>
+        <v>7.92</v>
       </c>
     </row>
     <row r="459" spans="1:20" x14ac:dyDescent="0.3">
@@ -11342,7 +11355,7 @@
         <v>44358</v>
       </c>
       <c r="G459">
-        <v>6.92</v>
+        <v>7.92</v>
       </c>
     </row>
     <row r="460" spans="1:20" x14ac:dyDescent="0.3">
@@ -11382,7 +11395,7 @@
         <v>44363</v>
       </c>
       <c r="G461">
-        <v>7.58</v>
+        <v>8.58</v>
       </c>
     </row>
     <row r="462" spans="1:20" x14ac:dyDescent="0.3">
@@ -11402,7 +11415,7 @@
         <v>44369</v>
       </c>
       <c r="G462">
-        <v>7.92</v>
+        <v>8.92</v>
       </c>
     </row>
     <row r="463" spans="1:20" x14ac:dyDescent="0.3">
@@ -11422,7 +11435,7 @@
         <v>44374</v>
       </c>
       <c r="G463">
-        <v>7.92</v>
+        <v>8.92</v>
       </c>
     </row>
     <row r="464" spans="1:20" x14ac:dyDescent="0.3">
@@ -11442,7 +11455,7 @@
         <v>44377</v>
       </c>
       <c r="G464">
-        <v>8.08</v>
+        <v>9.08</v>
       </c>
     </row>
     <row r="465" spans="1:20" x14ac:dyDescent="0.3">
@@ -11462,7 +11475,7 @@
         <v>44380</v>
       </c>
       <c r="G465">
-        <v>8.17</v>
+        <v>9.17</v>
       </c>
     </row>
     <row r="466" spans="1:20" x14ac:dyDescent="0.3">
@@ -11482,7 +11495,7 @@
         <v>44384</v>
       </c>
       <c r="G466">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="467" spans="1:20" x14ac:dyDescent="0.3">
@@ -11502,7 +11515,7 @@
         <v>44386</v>
       </c>
       <c r="G467">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="468" spans="1:20" x14ac:dyDescent="0.3">
@@ -11522,7 +11535,7 @@
         <v>44389</v>
       </c>
       <c r="G468">
-        <v>8.67</v>
+        <v>9.67</v>
       </c>
     </row>
     <row r="469" spans="1:20" x14ac:dyDescent="0.3">
@@ -11542,7 +11555,7 @@
         <v>44397</v>
       </c>
       <c r="G469">
-        <v>8.75</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="470" spans="1:20" x14ac:dyDescent="0.3">
@@ -11562,7 +11575,7 @@
         <v>44400</v>
       </c>
       <c r="G470">
-        <v>8.92</v>
+        <v>9.92</v>
       </c>
     </row>
     <row r="471" spans="1:20" x14ac:dyDescent="0.3">
@@ -11582,7 +11595,7 @@
         <v>44405</v>
       </c>
       <c r="G471">
-        <v>9.42</v>
+        <v>10.42</v>
       </c>
     </row>
     <row r="472" spans="1:20" x14ac:dyDescent="0.3">
@@ -11605,7 +11618,7 @@
         <v>9.2789999999999999</v>
       </c>
       <c r="G472">
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
       <c r="H472">
         <v>32</v>
@@ -11643,7 +11656,7 @@
         <v>44410</v>
       </c>
       <c r="G473">
-        <v>9.67</v>
+        <v>10.67</v>
       </c>
     </row>
     <row r="474" spans="1:20" x14ac:dyDescent="0.3">
@@ -11663,7 +11676,7 @@
         <v>44418</v>
       </c>
       <c r="G474">
-        <v>9.83</v>
+        <v>10.83</v>
       </c>
     </row>
     <row r="475" spans="1:20" x14ac:dyDescent="0.3">
@@ -11683,7 +11696,7 @@
         <v>44425</v>
       </c>
       <c r="G475">
-        <v>10.25</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="476" spans="1:20" x14ac:dyDescent="0.3">
@@ -11703,7 +11716,7 @@
         <v>44441</v>
       </c>
       <c r="G476">
-        <v>11.25</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="477" spans="1:20" x14ac:dyDescent="0.3">
@@ -11723,7 +11736,7 @@
         <v>44446</v>
       </c>
       <c r="G477">
-        <v>11.58</v>
+        <v>12.58</v>
       </c>
     </row>
     <row r="478" spans="1:20" x14ac:dyDescent="0.3">
@@ -11743,7 +11756,7 @@
         <v>44451</v>
       </c>
       <c r="G478">
-        <v>11.67</v>
+        <v>12.67</v>
       </c>
     </row>
     <row r="479" spans="1:20" x14ac:dyDescent="0.3">
@@ -11763,7 +11776,7 @@
         <v>44455</v>
       </c>
       <c r="G479">
-        <v>12.08</v>
+        <v>13.08</v>
       </c>
     </row>
     <row r="480" spans="1:20" x14ac:dyDescent="0.3">
@@ -11783,7 +11796,7 @@
         <v>44460</v>
       </c>
       <c r="G480">
-        <v>12.25</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="481" spans="1:20" x14ac:dyDescent="0.3">
@@ -11803,7 +11816,7 @@
         <v>44463</v>
       </c>
       <c r="G481">
-        <v>12.42</v>
+        <v>13.42</v>
       </c>
     </row>
     <row r="482" spans="1:20" x14ac:dyDescent="0.3">
@@ -11823,7 +11836,7 @@
         <v>44467</v>
       </c>
       <c r="G482">
-        <v>12.83</v>
+        <v>13.83</v>
       </c>
     </row>
     <row r="483" spans="1:20" x14ac:dyDescent="0.3">
@@ -11843,7 +11856,7 @@
         <v>44471</v>
       </c>
       <c r="G483">
-        <v>13.17</v>
+        <v>14.17</v>
       </c>
     </row>
     <row r="484" spans="1:20" x14ac:dyDescent="0.3">
@@ -11863,7 +11876,7 @@
         <v>44477</v>
       </c>
       <c r="G484">
-        <v>13.58</v>
+        <v>14.58</v>
       </c>
     </row>
     <row r="485" spans="1:20" x14ac:dyDescent="0.3">
@@ -11941,7 +11954,7 @@
         <v>44489</v>
       </c>
       <c r="G487">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="488" spans="1:20" x14ac:dyDescent="0.3">
@@ -12172,7 +12185,7 @@
         <v>44330</v>
       </c>
       <c r="G496">
-        <v>0.9</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="497" spans="1:20" x14ac:dyDescent="0.3">
@@ -12192,7 +12205,7 @@
         <v>44335</v>
       </c>
       <c r="G497">
-        <v>1.1000000000000001</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="498" spans="1:20" x14ac:dyDescent="0.3">
@@ -12212,7 +12225,7 @@
         <v>44337</v>
       </c>
       <c r="G498">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="499" spans="1:20" x14ac:dyDescent="0.3">
@@ -12232,7 +12245,7 @@
         <v>44342</v>
       </c>
       <c r="G499">
-        <v>1.9</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="500" spans="1:20" x14ac:dyDescent="0.3">
@@ -12252,7 +12265,7 @@
         <v>44345</v>
       </c>
       <c r="G500">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="501" spans="1:20" x14ac:dyDescent="0.3">
@@ -12272,7 +12285,7 @@
         <v>44350</v>
       </c>
       <c r="G501">
-        <v>2.7</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="502" spans="1:20" x14ac:dyDescent="0.3">
@@ -12292,7 +12305,7 @@
         <v>44355</v>
       </c>
       <c r="G502">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="503" spans="1:20" x14ac:dyDescent="0.3">
@@ -12350,7 +12363,7 @@
         <v>44358</v>
       </c>
       <c r="G504">
-        <v>3.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="505" spans="1:20" x14ac:dyDescent="0.3">
@@ -12370,7 +12383,7 @@
         <v>44362</v>
       </c>
       <c r="G505">
-        <v>3.7</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="506" spans="1:20" x14ac:dyDescent="0.3">
@@ -12390,7 +12403,7 @@
         <v>44369</v>
       </c>
       <c r="G506">
-        <v>4.0999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="507" spans="1:20" x14ac:dyDescent="0.3">
@@ -12410,7 +12423,7 @@
         <v>44374</v>
       </c>
       <c r="G507">
-        <v>4.4000000000000004</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="508" spans="1:20" x14ac:dyDescent="0.3">
@@ -12430,7 +12443,7 @@
         <v>44377</v>
       </c>
       <c r="G508">
-        <v>4.7</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="509" spans="1:20" x14ac:dyDescent="0.3">
@@ -12450,7 +12463,7 @@
         <v>44380</v>
       </c>
       <c r="G509">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="510" spans="1:20" x14ac:dyDescent="0.3">
@@ -12470,7 +12483,7 @@
         <v>44384</v>
       </c>
       <c r="G510">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="511" spans="1:20" x14ac:dyDescent="0.3">
@@ -12490,7 +12503,7 @@
         <v>44387</v>
       </c>
       <c r="G511">
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="512" spans="1:20" x14ac:dyDescent="0.3">
@@ -12510,7 +12523,7 @@
         <v>44390</v>
       </c>
       <c r="G512">
-        <v>5.3</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="513" spans="1:20" x14ac:dyDescent="0.3">
@@ -12530,7 +12543,7 @@
         <v>44398</v>
       </c>
       <c r="G513">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="514" spans="1:20" x14ac:dyDescent="0.3">
@@ -12550,7 +12563,7 @@
         <v>44403</v>
       </c>
       <c r="G514">
-        <v>6.2</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="515" spans="1:20" x14ac:dyDescent="0.3">
@@ -12570,7 +12583,7 @@
         <v>44407</v>
       </c>
       <c r="G515">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="516" spans="1:20" x14ac:dyDescent="0.3">
@@ -12590,7 +12603,7 @@
         <v>44412</v>
       </c>
       <c r="G516">
-        <v>6.7</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="517" spans="1:20" x14ac:dyDescent="0.3">
@@ -12610,7 +12623,7 @@
         <v>44418</v>
       </c>
       <c r="G517">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="518" spans="1:20" x14ac:dyDescent="0.3">
@@ -12630,7 +12643,7 @@
         <v>44425</v>
       </c>
       <c r="G518">
-        <v>7.4</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="519" spans="1:20" x14ac:dyDescent="0.3">
@@ -12653,7 +12666,7 @@
         <v>3.548</v>
       </c>
       <c r="G519">
-        <v>8.6</v>
+        <v>9.6</v>
       </c>
       <c r="H519">
         <v>30</v>
@@ -12691,7 +12704,7 @@
         <v>44446</v>
       </c>
       <c r="G520">
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="521" spans="1:20" x14ac:dyDescent="0.3">
@@ -12711,7 +12724,7 @@
         <v>44451</v>
       </c>
       <c r="G521">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="522" spans="1:20" x14ac:dyDescent="0.3">
@@ -12751,7 +12764,7 @@
         <v>44455</v>
       </c>
       <c r="G523">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="524" spans="1:20" x14ac:dyDescent="0.3">
@@ -12771,7 +12784,7 @@
         <v>44460</v>
       </c>
       <c r="G524">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="525" spans="1:20" x14ac:dyDescent="0.3">
@@ -12791,7 +12804,7 @@
         <v>44463</v>
       </c>
       <c r="G525">
-        <v>10.199999999999999</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="526" spans="1:20" x14ac:dyDescent="0.3">
@@ -12811,7 +12824,7 @@
         <v>44467</v>
       </c>
       <c r="G526">
-        <v>10.3</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="527" spans="1:20" x14ac:dyDescent="0.3">
@@ -12831,7 +12844,7 @@
         <v>44471</v>
       </c>
       <c r="G527">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="528" spans="1:20" x14ac:dyDescent="0.3">
@@ -12851,7 +12864,7 @@
         <v>44477</v>
       </c>
       <c r="G528">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="529" spans="1:20" x14ac:dyDescent="0.3">
@@ -12871,7 +12884,7 @@
         <v>44489</v>
       </c>
       <c r="G529">
-        <v>12.3</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="530" spans="1:20" x14ac:dyDescent="0.3">
@@ -12891,7 +12904,7 @@
         <v>44491</v>
       </c>
       <c r="G530">
-        <v>12.3</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="531" spans="1:20" x14ac:dyDescent="0.3">
@@ -12914,7 +12927,7 @@
         <v>9.2690000000000001</v>
       </c>
       <c r="G531">
-        <v>13.2</v>
+        <v>14.2</v>
       </c>
       <c r="H531">
         <v>40</v>
@@ -13200,7 +13213,7 @@
         <v>44379</v>
       </c>
       <c r="G542">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="543" spans="1:20" x14ac:dyDescent="0.3">
@@ -13220,7 +13233,7 @@
         <v>44384</v>
       </c>
       <c r="G543">
-        <v>0.17</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="544" spans="1:20" x14ac:dyDescent="0.3">
@@ -13240,7 +13253,7 @@
         <v>44387</v>
       </c>
       <c r="G544">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="545" spans="1:20" x14ac:dyDescent="0.3">
@@ -13260,7 +13273,7 @@
         <v>44390</v>
       </c>
       <c r="G545">
-        <v>0.33</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="546" spans="1:20" x14ac:dyDescent="0.3">
@@ -13280,7 +13293,7 @@
         <v>44398</v>
       </c>
       <c r="G546">
-        <v>1.17</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="547" spans="1:20" x14ac:dyDescent="0.3">
@@ -13300,7 +13313,7 @@
         <v>44403</v>
       </c>
       <c r="G547">
-        <v>1.58</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="548" spans="1:20" x14ac:dyDescent="0.3">
@@ -13320,7 +13333,7 @@
         <v>44407</v>
       </c>
       <c r="G548">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="549" spans="1:20" x14ac:dyDescent="0.3">
@@ -13378,7 +13391,7 @@
         <v>44412</v>
       </c>
       <c r="G550">
-        <v>2.17</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="551" spans="1:20" x14ac:dyDescent="0.3">
@@ -13398,7 +13411,7 @@
         <v>44418</v>
       </c>
       <c r="G551">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="552" spans="1:20" x14ac:dyDescent="0.3">
@@ -13418,7 +13431,7 @@
         <v>44425</v>
       </c>
       <c r="G552">
-        <v>3.33</v>
+        <v>4.33</v>
       </c>
     </row>
     <row r="553" spans="1:20" x14ac:dyDescent="0.3">
@@ -13438,7 +13451,7 @@
         <v>44441</v>
       </c>
       <c r="G553">
-        <v>4.92</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="554" spans="1:20" x14ac:dyDescent="0.3">
@@ -13458,7 +13471,7 @@
         <v>44446</v>
       </c>
       <c r="G554">
-        <v>5.25</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="555" spans="1:20" x14ac:dyDescent="0.3">
@@ -13478,7 +13491,7 @@
         <v>44451</v>
       </c>
       <c r="G555">
-        <v>5.83</v>
+        <v>6.83</v>
       </c>
     </row>
     <row r="556" spans="1:20" x14ac:dyDescent="0.3">
@@ -13498,7 +13511,7 @@
         <v>44455</v>
       </c>
       <c r="G556">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="557" spans="1:20" x14ac:dyDescent="0.3">
@@ -13518,7 +13531,7 @@
         <v>44460</v>
       </c>
       <c r="G557">
-        <v>6.33</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="558" spans="1:20" x14ac:dyDescent="0.3">
@@ -13541,7 +13554,7 @@
         <v>2.484</v>
       </c>
       <c r="G558">
-        <v>6.83</v>
+        <v>7.83</v>
       </c>
       <c r="H558">
         <v>30</v>
@@ -13579,7 +13592,7 @@
         <v>44467</v>
       </c>
       <c r="G559">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="560" spans="1:20" x14ac:dyDescent="0.3">
@@ -13599,7 +13612,7 @@
         <v>44471</v>
       </c>
       <c r="G560">
-        <v>7.33</v>
+        <v>8.33</v>
       </c>
       <c r="I560" t="s">
         <v>16</v>
@@ -13622,7 +13635,7 @@
         <v>44477</v>
       </c>
       <c r="G561">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="562" spans="1:20" x14ac:dyDescent="0.3">
@@ -13680,7 +13693,7 @@
         <v>44489</v>
       </c>
       <c r="G563">
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="564" spans="1:20" x14ac:dyDescent="0.3">
@@ -13700,7 +13713,7 @@
         <v>44491</v>
       </c>
       <c r="G564">
-        <v>9.58</v>
+        <v>10.58</v>
       </c>
     </row>
     <row r="565" spans="1:20" x14ac:dyDescent="0.3">
@@ -13720,7 +13733,7 @@
         <v>44496</v>
       </c>
       <c r="G565">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="566" spans="1:20" x14ac:dyDescent="0.3">
@@ -13740,7 +13753,7 @@
         <v>44499</v>
       </c>
       <c r="G566">
-        <v>10.75</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="567" spans="1:20" x14ac:dyDescent="0.3">
@@ -13760,7 +13773,7 @@
         <v>44503</v>
       </c>
       <c r="G567">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I567" t="s">
         <v>17</v>
@@ -13821,7 +13834,7 @@
         <v>44508</v>
       </c>
       <c r="G569">
-        <v>11.67</v>
+        <v>12.67</v>
       </c>
     </row>
     <row r="570" spans="1:20" x14ac:dyDescent="0.3">
@@ -14070,7 +14083,7 @@
         <v>44281</v>
       </c>
       <c r="G578">
-        <v>3.7</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="579" spans="1:20" x14ac:dyDescent="0.3">
@@ -14090,7 +14103,7 @@
         <v>44294</v>
       </c>
       <c r="G579">
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="580" spans="1:20" x14ac:dyDescent="0.3">
@@ -14110,7 +14123,7 @@
         <v>44301</v>
       </c>
       <c r="G580">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="581" spans="1:20" x14ac:dyDescent="0.3">
@@ -14130,7 +14143,7 @@
         <v>44303</v>
       </c>
       <c r="G581">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="582" spans="1:20" x14ac:dyDescent="0.3">
@@ -14150,7 +14163,7 @@
         <v>44306</v>
       </c>
       <c r="G582">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="583" spans="1:20" x14ac:dyDescent="0.3">
@@ -14170,7 +14183,7 @@
         <v>44311</v>
       </c>
       <c r="G583">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="584" spans="1:20" x14ac:dyDescent="0.3">
@@ -14190,7 +14203,7 @@
         <v>44314</v>
       </c>
       <c r="G584">
-        <v>7.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="585" spans="1:20" x14ac:dyDescent="0.3">
@@ -14210,7 +14223,7 @@
         <v>44316</v>
       </c>
       <c r="G585">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="586" spans="1:20" x14ac:dyDescent="0.3">
@@ -14230,7 +14243,7 @@
         <v>44322</v>
       </c>
       <c r="G586">
-        <v>7.7</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="587" spans="1:20" x14ac:dyDescent="0.3">
@@ -14250,7 +14263,7 @@
         <v>44327</v>
       </c>
       <c r="G587">
-        <v>8.1999999999999993</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="588" spans="1:20" x14ac:dyDescent="0.3">
@@ -14270,7 +14283,7 @@
         <v>44332</v>
       </c>
       <c r="G588">
-        <v>8.3000000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="589" spans="1:20" x14ac:dyDescent="0.3">
@@ -14290,7 +14303,7 @@
         <v>44335</v>
       </c>
       <c r="G589">
-        <v>8.6999999999999993</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="590" spans="1:20" x14ac:dyDescent="0.3">
@@ -14348,7 +14361,7 @@
         <v>44337</v>
       </c>
       <c r="G591">
-        <v>8.6999999999999993</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="592" spans="1:20" x14ac:dyDescent="0.3">
@@ -14368,7 +14381,7 @@
         <v>44342</v>
       </c>
       <c r="G592">
-        <v>8.8000000000000007</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="593" spans="1:20" x14ac:dyDescent="0.3">
@@ -14388,7 +14401,7 @@
         <v>44345</v>
       </c>
       <c r="G593">
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="594" spans="1:20" x14ac:dyDescent="0.3">
@@ -14428,7 +14441,7 @@
         <v>44352</v>
       </c>
       <c r="G595">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="596" spans="1:20" x14ac:dyDescent="0.3">
@@ -14448,7 +14461,7 @@
         <v>44356</v>
       </c>
       <c r="G596">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="597" spans="1:20" x14ac:dyDescent="0.3">
@@ -14468,7 +14481,7 @@
         <v>44359</v>
       </c>
       <c r="G597">
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="598" spans="1:20" x14ac:dyDescent="0.3">
@@ -14488,7 +14501,7 @@
         <v>44363</v>
       </c>
       <c r="G598">
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="599" spans="1:20" x14ac:dyDescent="0.3">
@@ -14511,7 +14524,7 @@
         <v>9.0410000000000004</v>
       </c>
       <c r="G599">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
       <c r="H599">
         <v>32</v>
@@ -14549,7 +14562,7 @@
         <v>44372</v>
       </c>
       <c r="G600">
-        <v>10.6</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="601" spans="1:20" x14ac:dyDescent="0.3">
@@ -14569,7 +14582,7 @@
         <v>44375</v>
       </c>
       <c r="G601">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="602" spans="1:20" x14ac:dyDescent="0.3">
@@ -14589,7 +14602,7 @@
         <v>44379</v>
       </c>
       <c r="G602">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="603" spans="1:20" x14ac:dyDescent="0.3">
@@ -14609,7 +14622,7 @@
         <v>44384</v>
       </c>
       <c r="G603">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="604" spans="1:20" x14ac:dyDescent="0.3">
@@ -14629,7 +14642,7 @@
         <v>44386</v>
       </c>
       <c r="G604">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="605" spans="1:20" x14ac:dyDescent="0.3">
@@ -14649,7 +14662,7 @@
         <v>44389</v>
       </c>
       <c r="G605">
-        <v>10.9</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="606" spans="1:20" x14ac:dyDescent="0.3">
@@ -14669,7 +14682,7 @@
         <v>44397</v>
       </c>
       <c r="G606">
-        <v>11.1</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="607" spans="1:20" x14ac:dyDescent="0.3">
@@ -14689,7 +14702,7 @@
         <v>44400</v>
       </c>
       <c r="G607">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="608" spans="1:20" x14ac:dyDescent="0.3">
@@ -14709,7 +14722,7 @@
         <v>44405</v>
       </c>
       <c r="G608">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="609" spans="1:20" x14ac:dyDescent="0.3">
@@ -14729,7 +14742,7 @@
         <v>44407</v>
       </c>
       <c r="G609">
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="610" spans="1:20" x14ac:dyDescent="0.3">
@@ -14749,7 +14762,7 @@
         <v>44410</v>
       </c>
       <c r="G610">
-        <v>11.9</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="611" spans="1:20" x14ac:dyDescent="0.3">
@@ -14769,7 +14782,7 @@
         <v>44418</v>
       </c>
       <c r="G611">
-        <v>12.3</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="612" spans="1:20" x14ac:dyDescent="0.3">
@@ -14789,7 +14802,7 @@
         <v>44425</v>
       </c>
       <c r="G612">
-        <v>12.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="613" spans="1:20" x14ac:dyDescent="0.3">
@@ -14809,7 +14822,7 @@
         <v>44441</v>
       </c>
       <c r="G613">
-        <v>13.8</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="614" spans="1:20" x14ac:dyDescent="0.3">
@@ -14829,7 +14842,7 @@
         <v>44446</v>
       </c>
       <c r="G614">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="615" spans="1:20" x14ac:dyDescent="0.3">
@@ -14849,7 +14862,7 @@
         <v>44451</v>
       </c>
       <c r="G615">
-        <v>14.2</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="616" spans="1:20" x14ac:dyDescent="0.3">
@@ -14869,7 +14882,7 @@
         <v>44455</v>
       </c>
       <c r="G616">
-        <v>14.4</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="617" spans="1:20" x14ac:dyDescent="0.3">
@@ -14889,7 +14902,7 @@
         <v>44460</v>
       </c>
       <c r="G617">
-        <v>14.8</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="618" spans="1:20" x14ac:dyDescent="0.3">
@@ -14909,7 +14922,7 @@
         <v>44463</v>
       </c>
       <c r="G618">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="619" spans="1:20" x14ac:dyDescent="0.3">
@@ -14929,7 +14942,7 @@
         <v>44467</v>
       </c>
       <c r="G619">
-        <v>15.2</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="620" spans="1:20" x14ac:dyDescent="0.3">
@@ -14949,7 +14962,7 @@
         <v>44471</v>
       </c>
       <c r="G620">
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="621" spans="1:20" x14ac:dyDescent="0.3">
@@ -14969,7 +14982,7 @@
         <v>44477</v>
       </c>
       <c r="G621">
-        <v>17.399999999999999</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="622" spans="1:20" x14ac:dyDescent="0.3">
@@ -15047,7 +15060,7 @@
         <v>44489</v>
       </c>
       <c r="G624">
-        <v>18.399999999999999</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="625" spans="1:20" x14ac:dyDescent="0.3">
@@ -15258,7 +15271,7 @@
         <v>44294</v>
       </c>
       <c r="G632">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="633" spans="1:20" x14ac:dyDescent="0.3">
@@ -15278,7 +15291,7 @@
         <v>44301</v>
       </c>
       <c r="G633">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="634" spans="1:20" x14ac:dyDescent="0.3">
@@ -15298,7 +15311,7 @@
         <v>44303</v>
       </c>
       <c r="G634">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="635" spans="1:20" x14ac:dyDescent="0.3">
@@ -15318,7 +15331,7 @@
         <v>44306</v>
       </c>
       <c r="G635">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="636" spans="1:20" x14ac:dyDescent="0.3">
@@ -15373,7 +15386,7 @@
         <v>44311</v>
       </c>
       <c r="G637">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="638" spans="1:20" x14ac:dyDescent="0.3">
@@ -15393,7 +15406,7 @@
         <v>44314</v>
       </c>
       <c r="G638">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="639" spans="1:20" x14ac:dyDescent="0.3">
@@ -15413,7 +15426,7 @@
         <v>44316</v>
       </c>
       <c r="G639">
-        <v>4.2</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="640" spans="1:20" x14ac:dyDescent="0.3">
@@ -15433,7 +15446,7 @@
         <v>44322</v>
       </c>
       <c r="G640">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="641" spans="1:20" x14ac:dyDescent="0.3">
@@ -15453,7 +15466,7 @@
         <v>44327</v>
       </c>
       <c r="G641">
-        <v>5.7</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="642" spans="1:20" x14ac:dyDescent="0.3">
@@ -15473,7 +15486,7 @@
         <v>44332</v>
       </c>
       <c r="G642">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="643" spans="1:20" x14ac:dyDescent="0.3">
@@ -15493,7 +15506,7 @@
         <v>44335</v>
       </c>
       <c r="G643">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="644" spans="1:20" x14ac:dyDescent="0.3">
@@ -15513,7 +15526,7 @@
         <v>44337</v>
       </c>
       <c r="G644">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="645" spans="1:20" x14ac:dyDescent="0.3">
@@ -15536,7 +15549,7 @@
         <v>4.7720000000000002</v>
       </c>
       <c r="G645">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
       <c r="H645">
         <v>30</v>
@@ -15574,7 +15587,7 @@
         <v>44345</v>
       </c>
       <c r="G646">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="647" spans="1:20" x14ac:dyDescent="0.3">
@@ -15594,7 +15607,7 @@
         <v>44352</v>
       </c>
       <c r="G647">
-        <v>6.7</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="648" spans="1:20" x14ac:dyDescent="0.3">
@@ -15614,7 +15627,7 @@
         <v>44355</v>
       </c>
       <c r="G648">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="649" spans="1:20" x14ac:dyDescent="0.3">
@@ -15634,7 +15647,7 @@
         <v>44358</v>
       </c>
       <c r="G649">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="650" spans="1:20" x14ac:dyDescent="0.3">
@@ -15674,7 +15687,7 @@
         <v>44363</v>
       </c>
       <c r="G651">
-        <v>7.6</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="652" spans="1:20" x14ac:dyDescent="0.3">
@@ -15694,7 +15707,7 @@
         <v>44369</v>
       </c>
       <c r="G652">
-        <v>7.6</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="653" spans="1:20" x14ac:dyDescent="0.3">
@@ -15714,7 +15727,7 @@
         <v>44374</v>
       </c>
       <c r="G653">
-        <v>8.3000000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="654" spans="1:20" x14ac:dyDescent="0.3">
@@ -15734,7 +15747,7 @@
         <v>44377</v>
       </c>
       <c r="G654">
-        <v>8.4</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="655" spans="1:20" x14ac:dyDescent="0.3">
@@ -15754,7 +15767,7 @@
         <v>44380</v>
       </c>
       <c r="G655">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="656" spans="1:20" x14ac:dyDescent="0.3">
@@ -15774,7 +15787,7 @@
         <v>44384</v>
       </c>
       <c r="G656">
-        <v>8.6</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="657" spans="1:20" x14ac:dyDescent="0.3">
@@ -15794,7 +15807,7 @@
         <v>44386</v>
       </c>
       <c r="G657">
-        <v>8.6</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="658" spans="1:20" x14ac:dyDescent="0.3">
@@ -15814,7 +15827,7 @@
         <v>44389</v>
       </c>
       <c r="G658">
-        <v>8.6</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="659" spans="1:20" x14ac:dyDescent="0.3">
@@ -15872,7 +15885,7 @@
         <v>44397</v>
       </c>
       <c r="G660">
-        <v>8.8000000000000007</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="661" spans="1:20" x14ac:dyDescent="0.3">
@@ -15892,7 +15905,7 @@
         <v>44400</v>
       </c>
       <c r="G661">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="662" spans="1:20" x14ac:dyDescent="0.3">
@@ -15912,7 +15925,7 @@
         <v>44405</v>
       </c>
       <c r="G662">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="663" spans="1:20" x14ac:dyDescent="0.3">
@@ -15932,7 +15945,7 @@
         <v>44407</v>
       </c>
       <c r="G663">
-        <v>9.6999999999999993</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="664" spans="1:20" x14ac:dyDescent="0.3">
@@ -15952,7 +15965,7 @@
         <v>44410</v>
       </c>
       <c r="G664">
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="665" spans="1:20" x14ac:dyDescent="0.3">
@@ -15972,7 +15985,7 @@
         <v>44418</v>
       </c>
       <c r="G665">
-        <v>10.4</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="666" spans="1:20" x14ac:dyDescent="0.3">
@@ -15992,7 +16005,7 @@
         <v>44425</v>
       </c>
       <c r="G666">
-        <v>10.6</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="667" spans="1:20" x14ac:dyDescent="0.3">
@@ -16012,7 +16025,7 @@
         <v>44441</v>
       </c>
       <c r="G667">
-        <v>11.4</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="668" spans="1:20" x14ac:dyDescent="0.3">
@@ -16032,7 +16045,7 @@
         <v>44446</v>
       </c>
       <c r="G668">
-        <v>11.6</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="669" spans="1:20" x14ac:dyDescent="0.3">
@@ -16052,7 +16065,7 @@
         <v>44451</v>
       </c>
       <c r="G669">
-        <v>11.8</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="670" spans="1:20" x14ac:dyDescent="0.3">
@@ -16072,7 +16085,7 @@
         <v>44455</v>
       </c>
       <c r="G670">
-        <v>12.1</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="671" spans="1:20" x14ac:dyDescent="0.3">
@@ -16092,7 +16105,7 @@
         <v>44460</v>
       </c>
       <c r="G671">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="672" spans="1:20" x14ac:dyDescent="0.3">
@@ -16112,7 +16125,7 @@
         <v>44463</v>
       </c>
       <c r="G672">
-        <v>12.6</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="673" spans="1:20" x14ac:dyDescent="0.3">
@@ -16132,7 +16145,7 @@
         <v>44467</v>
       </c>
       <c r="G673">
-        <v>12.8</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="674" spans="1:20" x14ac:dyDescent="0.3">
@@ -16152,7 +16165,7 @@
         <v>44471</v>
       </c>
       <c r="G674">
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="675" spans="1:20" x14ac:dyDescent="0.3">
@@ -16172,7 +16185,7 @@
         <v>44477</v>
       </c>
       <c r="G675">
-        <v>13.7</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="676" spans="1:20" x14ac:dyDescent="0.3">
@@ -16250,7 +16263,7 @@
         <v>44489</v>
       </c>
       <c r="G678">
-        <v>14.6</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="679" spans="1:20" x14ac:dyDescent="0.3">
@@ -16481,7 +16494,7 @@
         <v>44330</v>
       </c>
       <c r="G687">
-        <v>0.9</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="688" spans="1:20" x14ac:dyDescent="0.3">
@@ -16501,7 +16514,7 @@
         <v>44335</v>
       </c>
       <c r="G688">
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="689" spans="1:20" x14ac:dyDescent="0.3">
@@ -16521,7 +16534,7 @@
         <v>44337</v>
       </c>
       <c r="G689">
-        <v>1.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="690" spans="1:20" x14ac:dyDescent="0.3">
@@ -16541,7 +16554,7 @@
         <v>44342</v>
       </c>
       <c r="G690">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="691" spans="1:20" x14ac:dyDescent="0.3">
@@ -16561,7 +16574,7 @@
         <v>44345</v>
       </c>
       <c r="G691">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="692" spans="1:20" x14ac:dyDescent="0.3">
@@ -16581,7 +16594,7 @@
         <v>44350</v>
       </c>
       <c r="G692">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="693" spans="1:20" x14ac:dyDescent="0.3">
@@ -16601,7 +16614,7 @@
         <v>44355</v>
       </c>
       <c r="G693">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="694" spans="1:20" x14ac:dyDescent="0.3">
@@ -16659,7 +16672,7 @@
         <v>44358</v>
       </c>
       <c r="G695">
-        <v>3.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="696" spans="1:20" x14ac:dyDescent="0.3">
@@ -16679,7 +16692,7 @@
         <v>44362</v>
       </c>
       <c r="G696">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="697" spans="1:20" x14ac:dyDescent="0.3">
@@ -16699,7 +16712,7 @@
         <v>44369</v>
       </c>
       <c r="G697">
-        <v>4.4000000000000004</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="698" spans="1:20" x14ac:dyDescent="0.3">
@@ -16719,7 +16732,7 @@
         <v>44374</v>
       </c>
       <c r="G698">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="699" spans="1:20" x14ac:dyDescent="0.3">
@@ -16739,7 +16752,7 @@
         <v>44377</v>
       </c>
       <c r="G699">
-        <v>4.5999999999999996</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="700" spans="1:20" x14ac:dyDescent="0.3">
@@ -16759,7 +16772,7 @@
         <v>44380</v>
       </c>
       <c r="G700">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="701" spans="1:20" x14ac:dyDescent="0.3">
@@ -16779,7 +16792,7 @@
         <v>44384</v>
       </c>
       <c r="G701">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="702" spans="1:20" x14ac:dyDescent="0.3">
@@ -16799,7 +16812,7 @@
         <v>44387</v>
       </c>
       <c r="G702">
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="703" spans="1:20" x14ac:dyDescent="0.3">
@@ -16819,7 +16832,7 @@
         <v>44390</v>
       </c>
       <c r="G703">
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="704" spans="1:20" x14ac:dyDescent="0.3">
@@ -16839,7 +16852,7 @@
         <v>44398</v>
       </c>
       <c r="G704">
-        <v>5.6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="705" spans="1:20" x14ac:dyDescent="0.3">
@@ -16859,7 +16872,7 @@
         <v>44403</v>
       </c>
       <c r="G705">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="706" spans="1:20" x14ac:dyDescent="0.3">
@@ -16879,7 +16892,7 @@
         <v>44407</v>
       </c>
       <c r="G706">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="707" spans="1:20" x14ac:dyDescent="0.3">
@@ -16899,7 +16912,7 @@
         <v>44412</v>
       </c>
       <c r="G707">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="708" spans="1:20" x14ac:dyDescent="0.3">
@@ -16919,7 +16932,7 @@
         <v>44418</v>
       </c>
       <c r="G708">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="709" spans="1:20" x14ac:dyDescent="0.3">
@@ -16942,7 +16955,7 @@
         <v>3.3780000000000001</v>
       </c>
       <c r="G709">
-        <v>7.4</v>
+        <v>8.4</v>
       </c>
       <c r="H709">
         <v>30</v>
@@ -16980,7 +16993,7 @@
         <v>44441</v>
       </c>
       <c r="G710">
-        <v>8.4</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="711" spans="1:20" x14ac:dyDescent="0.3">
@@ -17038,7 +17051,7 @@
         <v>44446</v>
       </c>
       <c r="G712">
-        <v>8.8000000000000007</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I712" t="s">
         <v>16</v>
@@ -17061,7 +17074,7 @@
         <v>44451</v>
       </c>
       <c r="G713">
-        <v>8.9</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="714" spans="1:20" x14ac:dyDescent="0.3">
@@ -17081,7 +17094,7 @@
         <v>44455</v>
       </c>
       <c r="G714">
-        <v>9.3000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="715" spans="1:20" x14ac:dyDescent="0.3">
@@ -17101,7 +17114,7 @@
         <v>44460</v>
       </c>
       <c r="G715">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="716" spans="1:20" x14ac:dyDescent="0.3">
@@ -17121,7 +17134,7 @@
         <v>44463</v>
       </c>
       <c r="G716">
-        <v>9.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="717" spans="1:20" x14ac:dyDescent="0.3">
@@ -17141,7 +17154,7 @@
         <v>44467</v>
       </c>
       <c r="G717">
-        <v>10.199999999999999</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="718" spans="1:20" x14ac:dyDescent="0.3">
@@ -17161,7 +17174,7 @@
         <v>44471</v>
       </c>
       <c r="G718">
-        <v>10.4</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="719" spans="1:20" x14ac:dyDescent="0.3">
@@ -17181,7 +17194,7 @@
         <v>44477</v>
       </c>
       <c r="G719">
-        <v>10.9</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="720" spans="1:20" x14ac:dyDescent="0.3">
@@ -17201,7 +17214,7 @@
         <v>44489</v>
       </c>
       <c r="G720">
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="721" spans="1:20" x14ac:dyDescent="0.3">
@@ -17221,7 +17234,7 @@
         <v>44491</v>
       </c>
       <c r="G721">
-        <v>13.1</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="722" spans="1:20" x14ac:dyDescent="0.3">
@@ -17244,7 +17257,7 @@
         <v>11.329000000000001</v>
       </c>
       <c r="G722">
-        <v>13.7</v>
+        <v>14.7</v>
       </c>
       <c r="H722">
         <v>40</v>
@@ -17513,7 +17526,7 @@
         <v>44379</v>
       </c>
       <c r="G732">
-        <v>0.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="733" spans="1:20" x14ac:dyDescent="0.3">
@@ -17533,7 +17546,7 @@
         <v>44384</v>
       </c>
       <c r="G733">
-        <v>0.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="734" spans="1:20" x14ac:dyDescent="0.3">
@@ -17553,7 +17566,7 @@
         <v>44387</v>
       </c>
       <c r="G734">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="735" spans="1:20" x14ac:dyDescent="0.3">
@@ -17573,7 +17586,7 @@
         <v>44390</v>
       </c>
       <c r="G735">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="736" spans="1:20" x14ac:dyDescent="0.3">
@@ -17593,7 +17606,7 @@
         <v>44398</v>
       </c>
       <c r="G736">
-        <v>1.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="737" spans="1:20" x14ac:dyDescent="0.3">
@@ -17613,7 +17626,7 @@
         <v>44403</v>
       </c>
       <c r="G737">
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="738" spans="1:20" x14ac:dyDescent="0.3">
@@ -17633,7 +17646,7 @@
         <v>44407</v>
       </c>
       <c r="G738">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="739" spans="1:20" x14ac:dyDescent="0.3">
@@ -17688,7 +17701,7 @@
         <v>44412</v>
       </c>
       <c r="G740">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="741" spans="1:20" x14ac:dyDescent="0.3">
@@ -17708,7 +17721,7 @@
         <v>44418</v>
       </c>
       <c r="G741">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="742" spans="1:20" x14ac:dyDescent="0.3">
@@ -17728,7 +17741,7 @@
         <v>44425</v>
       </c>
       <c r="G742">
-        <v>3.9</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="743" spans="1:20" x14ac:dyDescent="0.3">
@@ -17748,7 +17761,7 @@
         <v>44441</v>
       </c>
       <c r="G743">
-        <v>5.6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="744" spans="1:20" x14ac:dyDescent="0.3">
@@ -17768,7 +17781,7 @@
         <v>44446</v>
       </c>
       <c r="G744">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="745" spans="1:20" x14ac:dyDescent="0.3">
@@ -17788,7 +17801,7 @@
         <v>44451</v>
       </c>
       <c r="G745">
-        <v>6.4</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="746" spans="1:20" x14ac:dyDescent="0.3">
@@ -17808,7 +17821,7 @@
         <v>44455</v>
       </c>
       <c r="G746">
-        <v>6.6</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="747" spans="1:20" x14ac:dyDescent="0.3">
@@ -17828,7 +17841,7 @@
         <v>44460</v>
       </c>
       <c r="G747">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="748" spans="1:20" x14ac:dyDescent="0.3">
@@ -17851,7 +17864,7 @@
         <v>2.8530000000000002</v>
       </c>
       <c r="G748">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="H748">
         <v>30</v>
@@ -17889,7 +17902,7 @@
         <v>44467</v>
       </c>
       <c r="G749">
-        <v>7.7</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="750" spans="1:20" x14ac:dyDescent="0.3">
@@ -17909,7 +17922,7 @@
         <v>44471</v>
       </c>
       <c r="G750">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I750" t="s">
         <v>16</v>
@@ -17932,7 +17945,7 @@
         <v>44477</v>
       </c>
       <c r="G751">
-        <v>8.6999999999999993</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="752" spans="1:20" x14ac:dyDescent="0.3">
@@ -17990,7 +18003,7 @@
         <v>44489</v>
       </c>
       <c r="G753">
-        <v>9.9</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="754" spans="1:21" x14ac:dyDescent="0.3">
@@ -18010,7 +18023,7 @@
         <v>44491</v>
       </c>
       <c r="G754">
-        <v>9.9</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="755" spans="1:21" x14ac:dyDescent="0.3">
@@ -18030,7 +18043,7 @@
         <v>44496</v>
       </c>
       <c r="G755">
-        <v>10.7</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="756" spans="1:21" x14ac:dyDescent="0.3">
@@ -18050,7 +18063,7 @@
         <v>44499</v>
       </c>
       <c r="G756">
-        <v>10.9</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="757" spans="1:21" x14ac:dyDescent="0.3">
@@ -18070,7 +18083,7 @@
         <v>44503</v>
       </c>
       <c r="G757">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
       <c r="I757" t="s">
         <v>17</v>
@@ -18131,7 +18144,7 @@
         <v>44508</v>
       </c>
       <c r="G759">
-        <v>11.8</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="760" spans="1:21" x14ac:dyDescent="0.3">
@@ -33006,7 +33019,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D1500" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing column name, SLN units,
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/Lincoln2021.xlsx
+++ b/Tests/Validation/Wheat/Lincoln2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E020A403-DC62-415B-836D-6CBA864D327B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F991B165-C6D4-4D83-BA2C-FB74CC5E7654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>NDVIModel.Script.NDVI</t>
   </si>
   <si>
-    <t>Wheat.Grain.GrainSize</t>
-  </si>
-  <si>
     <t>Wheat.Leaf.SpecificArea</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Wheat.Leaf.LAI</t>
+  </si>
+  <si>
+    <t>Wheat.Grain.Size</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1007,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,10 +1025,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>34</v>
@@ -1052,7 +1052,7 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>7</v>
@@ -1064,10 +1064,10 @@
         <v>9</v>
       </c>
       <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
         <v>36</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>37</v>
       </c>
       <c r="R1" t="s">
         <v>35</v>

</xml_diff>